<commit_message>
HW rev. 1 - finished routing, specified BOM, created gerbers
</commit_message>
<xml_diff>
--- a/eagle design/cos/Čos - POC - rectifier and zero cross detector - BOM.xlsx
+++ b/eagle design/cos/Čos - POC - rectifier and zero cross detector - BOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Čos - POC - rectifier and zero " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
   <si>
     <t>Qty</t>
   </si>
@@ -31,15 +31,6 @@
     <t>Parts</t>
   </si>
   <si>
-    <t>JP1Q</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>JP1, JP2, JP3, JP4, JP5, JP6, JP7, JP8</t>
-  </si>
-  <si>
     <t>100k</t>
   </si>
   <si>
@@ -176,13 +167,97 @@
   </si>
   <si>
     <t>mouser url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">833-SMBJ5356B-TP </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Micro-Commercial-Components-MCC/SMBJ5356B-TP?qs=%2Fha2pyFadujQlI%252Bovsu2dIVvji%2FULpZcaJMXGhg3YhPF3xL3ld2lcg%3D%3D</t>
+  </si>
+  <si>
+    <t>584-LT1716CS5#TRMPBF</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Analog-Devices/LT1716CS5TRMPBF?qs=%2Fha2pyFadujLvUfqpL8iAa57JmbvGUolaKsSySTrh2UECeK44kz9iw%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">849-LBA710S </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/IXYS-Integrated-Circuits/LBA710S?qs=8uBHJDVwVqzgfef1rN5c6w%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">621-DMN10H220L-7 </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Diodes-Incorporated/DMN10H220L-7?qs=%2Fha2pyFadui6aX5l%2FNbtt80qGfKcPMXPtfI6XoBbWY%252B41%2FteVg33rg%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">757-CUHS20S30H3F </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Toshiba/CUHS20S30H3F?qs=%2Fha2pyFadugVnzvuqBQjK7mNmFgLGyvkvvKthIvrsa6zTCxP3izpMQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">621-1N4148W-F </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Diodes-Incorporated/1N4148W-7-F?qs=%2Fha2pyFaduhvdRTUMUAPE5iMJ3chEEQ6fhH0Sc3FvyA%3D</t>
+  </si>
+  <si>
+    <t>647-UPW1V472MHD</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Nichicon/UPW1V472MHD?qs=%2Fha2pyFaduiERwYPL8c3nRShfDk4RNzwZqvNXmDlcV12MjtgXxrA6w%3D%3D</t>
+  </si>
+  <si>
+    <t>647-UHD1V331MPD</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Nichicon/UHD1V331MPD?qs=RhhqrI6N3g%2FaCcBAxpz5YQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">647-UHE1V332MHD6 </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Nichicon/UHE1V332MHD6?qs=%2Fha2pyFaduh%2FVvtnmOexBNcjzEqxV8XETiySkoDb%2Fy5n4ZjrNuYHaA%3D%3D</t>
+  </si>
+  <si>
+    <t>603-RT0805FRE0710KL</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE0710KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydi6xJ2%2FVOu7c%3D</t>
+  </si>
+  <si>
+    <t>603-RT0805BRD07100KL</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805BRD07100KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydbVwVVm%252B5HQE%3D</t>
+  </si>
+  <si>
+    <t>603-RT0805BRD0730KL</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805BRD0730KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydlJaovHNoOLo%3D</t>
+  </si>
+  <si>
+    <t>603-RT0805FRE0747K</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE0747KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydS35Dddwxr7g%3D</t>
+  </si>
+  <si>
+    <t>603-RT0805FRE10750RL</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE10750RL?qs=sGAEpiMZZMvdGkrng054tz3%252BeNFGeSG0b8vprN11rBqrXC%2Fny4PVvQ%3D%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +419,14 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -643,7 +726,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -686,12 +769,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -725,6 +813,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1025,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1038,7 +1127,8 @@
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="161.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1058,41 +1148,56 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1100,16 +1205,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1117,33 +1228,45 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1151,16 +1274,22 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1168,16 +1297,22 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>23</v>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1185,139 +1320,180 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>48</v>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G15" r:id="rId1"/>
+    <hyperlink ref="G14" r:id="rId2"/>
+    <hyperlink ref="G13" r:id="rId3"/>
+    <hyperlink ref="G12" r:id="rId4"/>
+    <hyperlink ref="G11" r:id="rId5"/>
+    <hyperlink ref="G4" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G7" r:id="rId8"/>
+    <hyperlink ref="G6" r:id="rId9"/>
+    <hyperlink ref="G3" r:id="rId10"/>
+    <hyperlink ref="G2" r:id="rId11"/>
+    <hyperlink ref="G5" r:id="rId12"/>
+    <hyperlink ref="G9" r:id="rId13"/>
+    <hyperlink ref="G10" r:id="rId14"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- corrected position in BOM
</commit_message>
<xml_diff>
--- a/eagle design/cos/Čos - POC - rectifier and zero cross detector - BOM.xlsx
+++ b/eagle design/cos/Čos - POC - rectifier and zero cross detector - BOM.xlsx
@@ -241,16 +241,16 @@
     <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805BRD0730KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydlJaovHNoOLo%3D</t>
   </si>
   <si>
-    <t>603-RT0805FRE0747K</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE0747KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydS35Dddwxr7g%3D</t>
-  </si>
-  <si>
     <t>603-RT0805FRE10750RL</t>
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE10750RL?qs=sGAEpiMZZMvdGkrng054tz3%252BeNFGeSG0b8vprN11rBqrXC%2Fny4PVvQ%3D%3D</t>
+  </si>
+  <si>
+    <t>603-RT0805FRE0747KL</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE0747KL?qs=%2Fha2pyFaduhFC1wu9jyUADMq3OpHh%252BVcLIGGOAj8K%2FkOFC1JonHvZN4lfpgCCLyX</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1117,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1332,10 +1332,10 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1355,10 +1355,10 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1490,10 +1490,9 @@
     <hyperlink ref="G3" r:id="rId10"/>
     <hyperlink ref="G2" r:id="rId11"/>
     <hyperlink ref="G5" r:id="rId12"/>
-    <hyperlink ref="G9" r:id="rId13"/>
-    <hyperlink ref="G10" r:id="rId14"/>
+    <hyperlink ref="G10" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- unified values of passive elements to a common format
</commit_message>
<xml_diff>
--- a/eagle design/cos/Čos - POC - rectifier and zero cross detector - BOM.xlsx
+++ b/eagle design/cos/Čos - POC - rectifier and zero cross detector - BOM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrvoje\Documents\vsite\MJ838 - cos components\eagle design\cos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12600"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>Qty</t>
   </si>
@@ -31,138 +36,42 @@
     <t>Parts</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>R-EU_R0805</t>
   </si>
   <si>
     <t>R0805</t>
   </si>
   <si>
-    <t>R2, R8</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>1N4148W-7-F</t>
-  </si>
-  <si>
-    <t>DIODE-SOD123</t>
-  </si>
-  <si>
-    <t>SOD123</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>30k</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
-    <t>C-POL</t>
-  </si>
-  <si>
-    <t>TH</t>
-  </si>
-  <si>
-    <t>C3, C4</t>
-  </si>
-  <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
-    <t>C5, C6</t>
-  </si>
-  <si>
     <t>47k</t>
   </si>
   <si>
-    <t>R7, R10</t>
-  </si>
-  <si>
-    <t>760R</t>
-  </si>
-  <si>
-    <t>R3, R4, R5, R6</t>
-  </si>
-  <si>
-    <t>CUHS20S30,H3F</t>
-  </si>
-  <si>
     <t>CUHS20S30</t>
   </si>
   <si>
     <t>US2H</t>
   </si>
   <si>
-    <t>D4, D5, D6, D7, D8</t>
-  </si>
-  <si>
-    <t>DMN10H220L-7</t>
-  </si>
-  <si>
     <t>MOSFET-NREFLOW</t>
   </si>
   <si>
     <t>SOT23</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
     <t>LBA710S</t>
   </si>
   <si>
     <t>LBA710</t>
   </si>
   <si>
-    <t>SMD_DIP6</t>
-  </si>
-  <si>
-    <t>IC2, IC3</t>
-  </si>
-  <si>
-    <t>LT1716CS5#TRMPBF</t>
-  </si>
-  <si>
-    <t>LT1716</t>
-  </si>
-  <si>
-    <t>TSOT-23</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>SMBJ5356B-TP</t>
-  </si>
-  <si>
-    <t>DIODE-DO214AA</t>
-  </si>
-  <si>
     <t>DO214AA</t>
   </si>
   <si>
-    <t>D1, D2</t>
-  </si>
-  <si>
-    <t>3300uF / 35V / ultralow ESR</t>
-  </si>
-  <si>
-    <t>330uF / 35V / ultralow ESR</t>
-  </si>
-  <si>
-    <t>4700uF / 35V / ultralow ESR</t>
-  </si>
-  <si>
     <t>mouser part no.</t>
   </si>
   <si>
@@ -172,92 +81,203 @@
     <t xml:space="preserve">833-SMBJ5356B-TP </t>
   </si>
   <si>
-    <t>https://hr.mouser.com/ProductDetail/Micro-Commercial-Components-MCC/SMBJ5356B-TP?qs=%2Fha2pyFadujQlI%252Bovsu2dIVvji%2FULpZcaJMXGhg3YhPF3xL3ld2lcg%3D%3D</t>
-  </si>
-  <si>
-    <t>584-LT1716CS5#TRMPBF</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Analog-Devices/LT1716CS5TRMPBF?qs=%2Fha2pyFadujLvUfqpL8iAa57JmbvGUolaKsSySTrh2UECeK44kz9iw%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">849-LBA710S </t>
   </si>
   <si>
-    <t>https://hr.mouser.com/ProductDetail/IXYS-Integrated-Circuits/LBA710S?qs=8uBHJDVwVqzgfef1rN5c6w%3D%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">621-DMN10H220L-7 </t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Diodes-Incorporated/DMN10H220L-7?qs=%2Fha2pyFadui6aX5l%2FNbtt80qGfKcPMXPtfI6XoBbWY%252B41%2FteVg33rg%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">757-CUHS20S30H3F </t>
   </si>
   <si>
-    <t>https://hr.mouser.com/ProductDetail/Toshiba/CUHS20S30H3F?qs=%2Fha2pyFadugVnzvuqBQjK7mNmFgLGyvkvvKthIvrsa6zTCxP3izpMQ%3D%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">621-1N4148W-F </t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Diodes-Incorporated/1N4148W-7-F?qs=%2Fha2pyFaduhvdRTUMUAPE5iMJ3chEEQ6fhH0Sc3FvyA%3D</t>
-  </si>
-  <si>
-    <t>647-UPW1V472MHD</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Nichicon/UPW1V472MHD?qs=%2Fha2pyFaduiERwYPL8c3nRShfDk4RNzwZqvNXmDlcV12MjtgXxrA6w%3D%3D</t>
-  </si>
-  <si>
-    <t>647-UHD1V331MPD</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Nichicon/UHD1V331MPD?qs=RhhqrI6N3g%2FaCcBAxpz5YQ%3D%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">647-UHE1V332MHD6 </t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Nichicon/UHE1V332MHD6?qs=%2Fha2pyFaduh%2FVvtnmOexBNcjzEqxV8XETiySkoDb%2Fy5n4ZjrNuYHaA%3D%3D</t>
-  </si>
-  <si>
-    <t>603-RT0805FRE0710KL</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE0710KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydi6xJ2%2FVOu7c%3D</t>
-  </si>
-  <si>
-    <t>603-RT0805BRD07100KL</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805BRD07100KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydbVwVVm%252B5HQE%3D</t>
-  </si>
-  <si>
-    <t>603-RT0805BRD0730KL</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805BRD0730KL?qs=sGAEpiMZZMvdGkrng054t%252BKCHBXLTLydlJaovHNoOLo%3D</t>
-  </si>
-  <si>
-    <t>603-RT0805FRE10750RL</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE10750RL?qs=sGAEpiMZZMvdGkrng054tz3%252BeNFGeSG0b8vprN11rBqrXC%2Fny4PVvQ%3D%3D</t>
-  </si>
-  <si>
-    <t>603-RT0805FRE0747KL</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Yageo/RT0805FRE0747KL?qs=%2Fha2pyFaduhFC1wu9jyUADMq3OpHh%252BVcLIGGOAj8K%2FkOFC1JonHvZN4lfpgCCLyX</t>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>C-EUC0805</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>C703</t>
+  </si>
+  <si>
+    <t>R121	 R122	 R221	 R222	 R321	 R322	 R421	 R422	 R521	 R522	 R702	 R707</t>
+  </si>
+  <si>
+    <t>10k/3W</t>
+  </si>
+  <si>
+    <t>R-EU_R2512</t>
+  </si>
+  <si>
+    <t>R2512</t>
+  </si>
+  <si>
+    <t>R701</t>
+  </si>
+  <si>
+    <t>10n/100v</t>
+  </si>
+  <si>
+    <t>C-EUC1812</t>
+  </si>
+  <si>
+    <t>C1812</t>
+  </si>
+  <si>
+    <t>C708</t>
+  </si>
+  <si>
+    <t>19V/5W</t>
+  </si>
+  <si>
+    <t>ZENER-DIODEDO214AA</t>
+  </si>
+  <si>
+    <t>D601	 D602</t>
+  </si>
+  <si>
+    <t>C902	 C907</t>
+  </si>
+  <si>
+    <t>430R/0.5W</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>6V/3W</t>
+  </si>
+  <si>
+    <t>D710</t>
+  </si>
+  <si>
+    <t>CUHS20S30	H3F</t>
+  </si>
+  <si>
+    <t>D1	 D2	 D3	 D4	 D808</t>
+  </si>
+  <si>
+    <t>IRLML2402TRPBF</t>
+  </si>
+  <si>
+    <t>Q102	 Q103	 Q202	 Q203	 Q302	 Q303	 Q402	 Q403	 Q502	 Q503</t>
+  </si>
+  <si>
+    <t>LAA710S</t>
+  </si>
+  <si>
+    <t>LAA710</t>
+  </si>
+  <si>
+    <t>SMD_DIP8</t>
+  </si>
+  <si>
+    <t>IC201	 IC401	 IC501</t>
+  </si>
+  <si>
+    <t>IC102	 IC302</t>
+  </si>
+  <si>
+    <t>LDK320AM33R</t>
+  </si>
+  <si>
+    <t>LDK320SOT-23-5L</t>
+  </si>
+  <si>
+    <t>SOT-23-5L</t>
+  </si>
+  <si>
+    <t>IC902</t>
+  </si>
+  <si>
+    <t>LT1638IDD#PBF</t>
+  </si>
+  <si>
+    <t>LT1638</t>
+  </si>
+  <si>
+    <t>DFN-8</t>
+  </si>
+  <si>
+    <t>IC701</t>
+  </si>
+  <si>
+    <t>1u / 10V</t>
+  </si>
+  <si>
+    <t>652-CHP2512JW103ELF</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/652-CHP2512JW103ELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C1812C104JDR </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/80-C1812C104JDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">942-IRLML2402TRPBF </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/942-IRLML2402TRPBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">584-LT1638IDD#PBF </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/584-LT1638IDD%23PBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">494-SMBJ5340BE3/TR13 </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/494-SMBJ5340BE3-TR13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77-VJ1812Y103JXEAT </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/77-VJ1812Y103JXEAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">849-LAA710S </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/849-LAA710S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">667-ERJ-P06F4300V </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/667-ERJ-P06F4300V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">581-08051C105K4T2A </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/581-08051C105K4T2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-LDK320AM33R </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/511-LDK320AM33R</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/833-SMBJ5356B-TP</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/849-LBA710S</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Toshiba/CUHS20S30H3F?qs=PqoDHHvF64%252BnIC9Qnnw9zg%3D%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,14 +439,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -726,7 +738,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -769,17 +781,12 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -813,7 +820,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -826,6 +832,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -872,7 +886,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -904,9 +918,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -938,6 +953,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1113,25 +1129,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="161.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,351 +1164,347 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>72</v>
+      <c r="E3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>68</v>
+      <c r="G6" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>64</v>
+        <v>75</v>
+      </c>
+      <c r="G8" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>52</v>
+      <c r="F16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G15" r:id="rId1"/>
-    <hyperlink ref="G14" r:id="rId2"/>
-    <hyperlink ref="G13" r:id="rId3"/>
-    <hyperlink ref="G12" r:id="rId4"/>
-    <hyperlink ref="G11" r:id="rId5"/>
-    <hyperlink ref="G4" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G7" r:id="rId8"/>
-    <hyperlink ref="G6" r:id="rId9"/>
-    <hyperlink ref="G3" r:id="rId10"/>
-    <hyperlink ref="G2" r:id="rId11"/>
-    <hyperlink ref="G5" r:id="rId12"/>
-    <hyperlink ref="G10" r:id="rId13"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>